<commit_message>
List all vegetables and fruits in alphabetic order (name the bottom tab "Fruits and Vegi" and color the tab blue)
</commit_message>
<xml_diff>
--- a/fruits and vegetables.xlsx
+++ b/fruits and vegetables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Fruits and Vegi" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -199,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -213,6 +213,11 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -231,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -246,11 +251,22 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF0B8043"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -455,6 +471,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
+    <tabColor rgb="FF0000FF"/>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -2375,16 +2392,61 @@
       <c r="B45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="4">
-        <f t="shared" ref="C45:D45" si="1">SUM(C2:C43)</f>
+      <c r="C45" s="6">
+        <f t="shared" ref="C45:N45" si="1">SUM(C2:C43)</f>
         <v>156.75</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="6">
         <f t="shared" si="1"/>
         <v>179</v>
       </c>
+      <c r="E45" s="6">
+        <f t="shared" si="1"/>
+        <v>171</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" si="1"/>
+        <v>162.5</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="1"/>
+        <v>167</v>
+      </c>
+      <c r="H45" s="6">
+        <f t="shared" si="1"/>
+        <v>192.5</v>
+      </c>
+      <c r="I45" s="6">
+        <f t="shared" si="1"/>
+        <v>174.25</v>
+      </c>
+      <c r="J45" s="6">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="K45" s="6">
+        <f t="shared" si="1"/>
+        <v>195.25</v>
+      </c>
+      <c r="L45" s="6">
+        <f t="shared" si="1"/>
+        <v>207.25</v>
+      </c>
+      <c r="M45" s="6">
+        <f t="shared" si="1"/>
+        <v>211.5</v>
+      </c>
+      <c r="N45" s="6">
+        <f t="shared" si="1"/>
+        <v>257</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B43">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>SORT(B2:B43)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>